<commit_message>
fix: change excel file
</commit_message>
<xml_diff>
--- a/public/exemple/exemple.xlsx
+++ b/public/exemple/exemple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camille.martin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E09D153-D6EF-4E6A-BE05-A264C480546F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDB09D3-46F4-4F7A-B32F-21722B5CDB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="133">
   <si>
     <t>GTINs/EANS</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Référence interne</t>
   </si>
   <si>
-    <t>Marque</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
@@ -238,30 +235,6 @@
     <t>Part du transport aérien</t>
   </si>
   <si>
-    <t>Accessoire 1</t>
-  </si>
-  <si>
-    <t>Accessoire 1 quantité</t>
-  </si>
-  <si>
-    <t>Accessoire 2</t>
-  </si>
-  <si>
-    <t>Accessoire 2 quantité</t>
-  </si>
-  <si>
-    <t>Accessoire 3</t>
-  </si>
-  <si>
-    <t>Accessoire 3 quantité</t>
-  </si>
-  <si>
-    <t>Accessoire 4</t>
-  </si>
-  <si>
-    <t>Accessoire 4 quantité</t>
-  </si>
-  <si>
     <t>1234567891000;1234567891001</t>
   </si>
   <si>
@@ -449,6 +422,21 @@
   </si>
   <si>
     <t>non</t>
+  </si>
+  <si>
+    <t>Marque ID</t>
+  </si>
+  <si>
+    <t>Quantité de bouton en métal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quantité de bouton en plastique</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quantité de zip long</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quantité de zip court</t>
   </si>
 </sst>
 </file>
@@ -832,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BV2"/>
+  <dimension ref="A1:BR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BG3" sqref="BG3"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BQ1" sqref="BQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14"/>
@@ -893,18 +881,11 @@
     <col min="63" max="63" width="15.75" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="16" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="11" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="11" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="11" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="18.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74">
+    <row r="1" spans="1:70">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,240 +893,228 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:70" ht="28">
+      <c r="A2" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="B2" t="s">
         <v>66</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:74" ht="28">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
       </c>
       <c r="D2">
         <v>2318</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F2">
         <v>0.55000000000000004</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H2">
         <v>9000</v>
@@ -1154,51 +1123,48 @@
         <v>100</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="L2" s="2">
         <v>0.9</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="N2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="O2" s="2">
         <v>0.1</v>
       </c>
       <c r="BG2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BH2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BI2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BJ2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="BK2" s="2">
         <v>0.2</v>
       </c>
       <c r="BL2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BM2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="BN2" s="3">
         <v>0.75</v>
       </c>
-      <c r="BO2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BP2">
+      <c r="BO2">
         <v>1</v>
       </c>
     </row>
@@ -1206,7 +1172,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83052150-8577-4F3C-8925-8A462BAB918A}">
           <x14:formula1>
             <xm:f>Valeurs!$A$2:$A$12</xm:f>
@@ -1224,12 +1190,6 @@
             <xm:f>Valeurs!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>BJ2:BJ1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD9E588E-34AA-4D09-91BB-38D17993C802}">
-          <x14:formula1>
-            <xm:f>Valeurs!$G$2:$G$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>BQ2:BQ1048576 BS2:BS1048576 BU2:BU1048576 BO2:BO1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B06D0A55-0ED9-462C-ACBE-689C63B026B0}">
           <x14:formula1>
@@ -1275,238 +1235,238 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
         <v>82</v>
-      </c>
-      <c r="G2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
         <v>88</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="D13" s="4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="D14" s="4" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="D15" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="D16" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="4:5">
       <c r="D17" s="4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E17" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="4:5">
       <c r="D18" s="4" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E18" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="4:5">
       <c r="E19" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="4:5">
       <c r="E20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="4:5">
       <c r="E21" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: change excel file (#72)
</commit_message>
<xml_diff>
--- a/public/exemple/exemple.xlsx
+++ b/public/exemple/exemple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camille.martin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E09D153-D6EF-4E6A-BE05-A264C480546F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEDB09D3-46F4-4F7A-B32F-21722B5CDB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="133">
   <si>
     <t>GTINs/EANS</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Référence interne</t>
   </si>
   <si>
-    <t>Marque</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
@@ -238,30 +235,6 @@
     <t>Part du transport aérien</t>
   </si>
   <si>
-    <t>Accessoire 1</t>
-  </si>
-  <si>
-    <t>Accessoire 1 quantité</t>
-  </si>
-  <si>
-    <t>Accessoire 2</t>
-  </si>
-  <si>
-    <t>Accessoire 2 quantité</t>
-  </si>
-  <si>
-    <t>Accessoire 3</t>
-  </si>
-  <si>
-    <t>Accessoire 3 quantité</t>
-  </si>
-  <si>
-    <t>Accessoire 4</t>
-  </si>
-  <si>
-    <t>Accessoire 4 quantité</t>
-  </si>
-  <si>
     <t>1234567891000;1234567891001</t>
   </si>
   <si>
@@ -449,6 +422,21 @@
   </si>
   <si>
     <t>non</t>
+  </si>
+  <si>
+    <t>Marque ID</t>
+  </si>
+  <si>
+    <t>Quantité de bouton en métal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quantité de bouton en plastique</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quantité de zip long</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quantité de zip court</t>
   </si>
 </sst>
 </file>
@@ -832,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BV2"/>
+  <dimension ref="A1:BR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BG3" sqref="BG3"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BQ1" sqref="BQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14"/>
@@ -893,18 +881,11 @@
     <col min="63" max="63" width="15.75" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="16" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="11" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11" bestFit="1" customWidth="1"/>
+    <col min="67" max="70" width="11" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="11" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="11" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="18.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74">
+    <row r="1" spans="1:70">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -912,240 +893,228 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BO1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:70" ht="28">
+      <c r="A2" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="B2" t="s">
         <v>66</v>
-      </c>
-      <c r="BP1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:74" ht="28">
-      <c r="A2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" t="s">
-        <v>75</v>
       </c>
       <c r="D2">
         <v>2318</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F2">
         <v>0.55000000000000004</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="H2">
         <v>9000</v>
@@ -1154,51 +1123,48 @@
         <v>100</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="L2" s="2">
         <v>0.9</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="N2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="O2" s="2">
         <v>0.1</v>
       </c>
       <c r="BG2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BH2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BI2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BJ2" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="BK2" s="2">
         <v>0.2</v>
       </c>
       <c r="BL2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="BM2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="BN2" s="3">
         <v>0.75</v>
       </c>
-      <c r="BO2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BP2">
+      <c r="BO2">
         <v>1</v>
       </c>
     </row>
@@ -1206,7 +1172,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83052150-8577-4F3C-8925-8A462BAB918A}">
           <x14:formula1>
             <xm:f>Valeurs!$A$2:$A$12</xm:f>
@@ -1224,12 +1190,6 @@
             <xm:f>Valeurs!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>BJ2:BJ1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CD9E588E-34AA-4D09-91BB-38D17993C802}">
-          <x14:formula1>
-            <xm:f>Valeurs!$G$2:$G$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>BQ2:BQ1048576 BS2:BS1048576 BU2:BU1048576 BO2:BO1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B06D0A55-0ED9-462C-ACBE-689C63B026B0}">
           <x14:formula1>
@@ -1275,238 +1235,238 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
         <v>82</v>
-      </c>
-      <c r="G2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s">
         <v>88</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="28">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="28">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="E10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="D13" s="4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="D14" s="4" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="D15" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="D16" s="4" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="4:5">
       <c r="D17" s="4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E17" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="4:5">
       <c r="D18" s="4" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="E18" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="4:5">
       <c r="E19" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="4:5">
       <c r="E20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="4:5">
       <c r="E21" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>